<commit_message>
[add] task session flow
</commit_message>
<xml_diff>
--- a/employees-list.xlsx
+++ b/employees-list.xlsx
@@ -20,45 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
   <si>
-    <t xml:space="preserve">EmployeeCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fullname</t>
   </si>
   <si>
     <t xml:space="preserve">Phone Number</t>
   </si>
   <si>
-    <t xml:space="preserve">BinhPham</t>
-  </si>
-  <si>
-    <t xml:space="preserve">binh@pham.com</t>
+    <t xml:space="preserve">RoleId</t>
   </si>
   <si>
     <t xml:space="preserve">Pham Duc Binh</t>
   </si>
   <si>
-    <t xml:space="preserve">DucPhi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">duc@phi.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Phi Do Hong Duc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocTran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc@tran.com</t>
   </si>
   <si>
     <t xml:space="preserve">Tran Thien Loc</t>
@@ -172,20 +151,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.95"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="4" style="1" width="11.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -201,25 +179,19 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="n">
         <v>321456789</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -227,16 +199,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>456123789</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,16 +213,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>987456123</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bulk register and delete api role check
</commit_message>
<xml_diff>
--- a/employees-list.xlsx
+++ b/employees-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Capstone\esms-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7763C4D-EB12-40A2-A2F8-7E9D9363DE2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0646C5-8F04-4931-AA1F-883B8F4C629F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24708" yWindow="1296" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>No.</t>
   </si>
@@ -39,16 +39,31 @@
     <t>Pham Duc Binh</t>
   </si>
   <si>
-    <t>Role id</t>
-  </si>
-  <si>
-    <t>Counter Id</t>
-  </si>
-  <si>
-    <t>Avatar Url</t>
-  </si>
-  <si>
     <t>Tran Thien Loc</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Bank teller</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Nguyen Phuoc An</t>
+  </si>
+  <si>
+    <t>0908063465</t>
+  </si>
+  <si>
+    <t>0908398763</t>
+  </si>
+  <si>
+    <t>0123567895</t>
   </si>
 </sst>
 </file>
@@ -95,7 +110,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMH4"/>
+  <dimension ref="A1:ALW4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -421,11 +438,11 @@
     <col min="1" max="1" width="11.5546875" style="1"/>
     <col min="2" max="2" width="33.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="1022" width="11.5546875" style="1"/>
-    <col min="1023" max="1025" width="11.5546875"/>
+    <col min="4" max="1011" width="11.5546875" style="1"/>
+    <col min="1012" max="1014" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,52 +453,50 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
-        <v>321456789</v>
-      </c>
-      <c r="D2" s="1">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3">
-        <v>3</v>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2">
-        <v>345646789</v>
-      </c>
-      <c r="D3" s="1">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3">
         <v>4</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>